<commit_message>
start point, all adjusted to Team class
</commit_message>
<xml_diff>
--- a/players_excel.xlsx
+++ b/players_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Shirt number</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>speed</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>agility</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>creating</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>shooting</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>stability</t>
         </is>
@@ -486,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Glenda</t>
+          <t>Fannie</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -494,23 +499,28 @@
           <t>Team A</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>62</v>
-      </c>
       <c r="F2" t="n">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="G2" t="n">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="H2" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I2" t="n">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="J2" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -519,7 +529,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Carolyn</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -527,23 +537,28 @@
           <t>Team A</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
-        <v>43</v>
-      </c>
       <c r="F3" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G3" t="n">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H3" t="n">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="I3" t="n">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="J3" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -552,7 +567,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Oscar</t>
+          <t>Lauren</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -560,23 +575,28 @@
           <t>Team A</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
-        <v>61</v>
-      </c>
       <c r="F4" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G4" t="n">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="H4" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I4" t="n">
-        <v>63</v>
+        <v>78</v>
+      </c>
+      <c r="J4" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -585,7 +605,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Josephine</t>
+          <t>Holly</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -593,23 +613,28 @@
           <t>Team A</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
-        <v>51</v>
-      </c>
       <c r="F5" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G5" t="n">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="H5" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="I5" t="n">
-        <v>48</v>
+        <v>77</v>
+      </c>
+      <c r="J5" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -618,7 +643,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Wayne</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -626,23 +651,28 @@
           <t>Team A</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="n">
-        <v>52</v>
-      </c>
       <c r="F6" t="n">
+        <v>71</v>
+      </c>
+      <c r="G6" t="n">
+        <v>67</v>
+      </c>
+      <c r="H6" t="n">
         <v>60</v>
       </c>
-      <c r="G6" t="n">
-        <v>54</v>
-      </c>
-      <c r="H6" t="n">
-        <v>66</v>
-      </c>
       <c r="I6" t="n">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="J6" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="7">
@@ -651,7 +681,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>Shayna</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -659,23 +689,28 @@
           <t>Team B</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
+        <v>46</v>
+      </c>
+      <c r="G7" t="n">
         <v>53</v>
       </c>
-      <c r="F7" t="n">
-        <v>69</v>
-      </c>
-      <c r="G7" t="n">
-        <v>65</v>
-      </c>
       <c r="H7" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I7" t="n">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="J7" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
@@ -684,7 +719,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bernadine</t>
+          <t>Howard</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -692,23 +727,28 @@
           <t>Team B</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="E8" t="n">
-        <v>71</v>
-      </c>
       <c r="F8" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="G8" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I8" t="n">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="J8" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -717,7 +757,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sara</t>
+          <t>Deloris</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -725,23 +765,28 @@
           <t>Team B</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>3</v>
       </c>
-      <c r="E9" t="n">
-        <v>63</v>
-      </c>
       <c r="F9" t="n">
+        <v>72</v>
+      </c>
+      <c r="G9" t="n">
         <v>56</v>
       </c>
-      <c r="G9" t="n">
-        <v>61</v>
-      </c>
       <c r="H9" t="n">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="I9" t="n">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="J9" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -750,7 +795,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -758,23 +803,28 @@
           <t>Team B</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>4</v>
       </c>
-      <c r="E10" t="n">
-        <v>65</v>
-      </c>
       <c r="F10" t="n">
+        <v>47</v>
+      </c>
+      <c r="G10" t="n">
+        <v>74</v>
+      </c>
+      <c r="H10" t="n">
+        <v>72</v>
+      </c>
+      <c r="I10" t="n">
+        <v>58</v>
+      </c>
+      <c r="J10" t="n">
         <v>71</v>
-      </c>
-      <c r="G10" t="n">
-        <v>61</v>
-      </c>
-      <c r="H10" t="n">
-        <v>56</v>
-      </c>
-      <c r="I10" t="n">
-        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -783,7 +833,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wayne</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -791,23 +841,28 @@
           <t>Team B</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>5</v>
       </c>
-      <c r="E11" t="n">
-        <v>69</v>
-      </c>
       <c r="F11" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" t="n">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="H11" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I11" t="n">
         <v>73</v>
+      </c>
+      <c r="J11" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -816,7 +871,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Julie</t>
+          <t>Phyllis</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -824,23 +879,28 @@
           <t>Team C</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>1</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
+        <v>69</v>
+      </c>
+      <c r="G12" t="n">
+        <v>57</v>
+      </c>
+      <c r="H12" t="n">
+        <v>43</v>
+      </c>
+      <c r="I12" t="n">
+        <v>56</v>
+      </c>
+      <c r="J12" t="n">
         <v>58</v>
-      </c>
-      <c r="F12" t="n">
-        <v>41</v>
-      </c>
-      <c r="G12" t="n">
-        <v>55</v>
-      </c>
-      <c r="H12" t="n">
-        <v>61</v>
-      </c>
-      <c r="I12" t="n">
-        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -849,7 +909,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ramona</t>
+          <t>Felipe</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -857,23 +917,28 @@
           <t>Team C</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>2</v>
       </c>
-      <c r="E13" t="n">
-        <v>64</v>
-      </c>
       <c r="F13" t="n">
+        <v>60</v>
+      </c>
+      <c r="G13" t="n">
+        <v>62</v>
+      </c>
+      <c r="H13" t="n">
         <v>46</v>
       </c>
-      <c r="G13" t="n">
-        <v>76</v>
-      </c>
-      <c r="H13" t="n">
-        <v>83</v>
-      </c>
       <c r="I13" t="n">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="J13" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="14">
@@ -882,7 +947,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Betty</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -890,23 +955,28 @@
           <t>Team C</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
         <v>3</v>
       </c>
-      <c r="E14" t="n">
-        <v>60</v>
-      </c>
       <c r="F14" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G14" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="H14" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I14" t="n">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="J14" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -915,7 +985,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Ida</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -923,23 +993,28 @@
           <t>Team C</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>4</v>
       </c>
-      <c r="E15" t="n">
-        <v>66</v>
-      </c>
       <c r="F15" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G15" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H15" t="n">
+        <v>63</v>
+      </c>
+      <c r="I15" t="n">
+        <v>57</v>
+      </c>
+      <c r="J15" t="n">
         <v>58</v>
-      </c>
-      <c r="I15" t="n">
-        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -948,7 +1023,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Eddie</t>
+          <t>Crystal</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -956,23 +1031,28 @@
           <t>Team C</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>5</v>
       </c>
-      <c r="E16" t="n">
-        <v>58</v>
-      </c>
       <c r="F16" t="n">
+        <v>62</v>
+      </c>
+      <c r="G16" t="n">
+        <v>43</v>
+      </c>
+      <c r="H16" t="n">
+        <v>70</v>
+      </c>
+      <c r="I16" t="n">
+        <v>67</v>
+      </c>
+      <c r="J16" t="n">
         <v>49</v>
-      </c>
-      <c r="G16" t="n">
-        <v>66</v>
-      </c>
-      <c r="H16" t="n">
-        <v>54</v>
-      </c>
-      <c r="I16" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +1061,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Ebony</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -989,23 +1069,28 @@
           <t>Team D</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>1</v>
       </c>
-      <c r="E17" t="n">
-        <v>60</v>
-      </c>
       <c r="F17" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G17" t="n">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="H17" t="n">
+        <v>68</v>
+      </c>
+      <c r="I17" t="n">
         <v>52</v>
       </c>
-      <c r="I17" t="n">
-        <v>48</v>
+      <c r="J17" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="18">
@@ -1014,7 +1099,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Billie</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1022,23 +1107,28 @@
           <t>Team D</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
         <v>2</v>
       </c>
-      <c r="E18" t="n">
-        <v>66</v>
-      </c>
       <c r="F18" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G18" t="n">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H18" t="n">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="I18" t="n">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="J18" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -1047,7 +1137,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Luz</t>
+          <t>Rachel</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1055,23 +1145,28 @@
           <t>Team D</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>3</v>
       </c>
-      <c r="E19" t="n">
-        <v>59</v>
-      </c>
       <c r="F19" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G19" t="n">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="H19" t="n">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="I19" t="n">
-        <v>58</v>
+        <v>82</v>
+      </c>
+      <c r="J19" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="20">
@@ -1080,7 +1175,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Clifford</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1088,23 +1183,28 @@
           <t>Team D</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>4</v>
       </c>
-      <c r="E20" t="n">
-        <v>53</v>
-      </c>
       <c r="F20" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H20" t="n">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="I20" t="n">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="J20" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="21">
@@ -1113,7 +1213,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Terry</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1121,23 +1221,28 @@
           <t>Team D</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>5</v>
       </c>
-      <c r="E21" t="n">
-        <v>57</v>
-      </c>
       <c r="F21" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G21" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="H21" t="n">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="I21" t="n">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="J21" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="22">
@@ -1146,7 +1251,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lizbeth</t>
+          <t>Jacob</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1154,23 +1259,28 @@
           <t>Team E</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>magenta</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>1</v>
       </c>
-      <c r="E22" t="n">
-        <v>65</v>
-      </c>
       <c r="F22" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G22" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="H22" t="n">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="I22" t="n">
-        <v>63</v>
+        <v>41</v>
+      </c>
+      <c r="J22" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -1179,7 +1289,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Donna</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1187,23 +1297,28 @@
           <t>Team E</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>magenta</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>2</v>
-      </c>
-      <c r="E23" t="n">
-        <v>74</v>
       </c>
       <c r="F23" t="n">
         <v>72</v>
       </c>
       <c r="G23" t="n">
+        <v>73</v>
+      </c>
+      <c r="H23" t="n">
+        <v>71</v>
+      </c>
+      <c r="I23" t="n">
         <v>53</v>
       </c>
-      <c r="H23" t="n">
-        <v>43</v>
-      </c>
-      <c r="I23" t="n">
-        <v>69</v>
+      <c r="J23" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="24">
@@ -1212,7 +1327,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Deborah</t>
+          <t>Victoria</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1220,23 +1335,28 @@
           <t>Team E</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>magenta</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
         <v>3</v>
       </c>
-      <c r="E24" t="n">
-        <v>67</v>
-      </c>
       <c r="F24" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G24" t="n">
+        <v>63</v>
+      </c>
+      <c r="H24" t="n">
+        <v>77</v>
+      </c>
+      <c r="I24" t="n">
+        <v>54</v>
+      </c>
+      <c r="J24" t="n">
         <v>59</v>
-      </c>
-      <c r="H24" t="n">
-        <v>54</v>
-      </c>
-      <c r="I24" t="n">
-        <v>47</v>
       </c>
     </row>
     <row r="25">
@@ -1245,7 +1365,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jared</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1253,23 +1373,28 @@
           <t>Team E</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>magenta</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>4</v>
       </c>
-      <c r="E25" t="n">
-        <v>70</v>
-      </c>
       <c r="F25" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G25" t="n">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H25" t="n">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="I25" t="n">
-        <v>75</v>
+        <v>53</v>
+      </c>
+      <c r="J25" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="26">
@@ -1278,7 +1403,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1286,23 +1411,28 @@
           <t>Team E</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>magenta</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
         <v>5</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
+        <v>71</v>
+      </c>
+      <c r="G26" t="n">
+        <v>56</v>
+      </c>
+      <c r="H26" t="n">
         <v>50</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>60</v>
       </c>
-      <c r="G26" t="n">
-        <v>65</v>
-      </c>
-      <c r="H26" t="n">
-        <v>65</v>
-      </c>
-      <c r="I26" t="n">
-        <v>82</v>
+      <c r="J26" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="27">
@@ -1311,7 +1441,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1319,23 +1449,28 @@
           <t>Team F</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>1</v>
       </c>
-      <c r="E27" t="n">
-        <v>72</v>
-      </c>
       <c r="F27" t="n">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G27" t="n">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="H27" t="n">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I27" t="n">
-        <v>69</v>
+        <v>36</v>
+      </c>
+      <c r="J27" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -1344,7 +1479,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bertha</t>
+          <t>Christine</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1352,23 +1487,28 @@
           <t>Team F</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>2</v>
       </c>
-      <c r="E28" t="n">
-        <v>48</v>
-      </c>
       <c r="F28" t="n">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G28" t="n">
+        <v>64</v>
+      </c>
+      <c r="H28" t="n">
         <v>58</v>
       </c>
-      <c r="H28" t="n">
-        <v>60</v>
-      </c>
       <c r="I28" t="n">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="J28" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="29">
@@ -1377,7 +1517,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Hope</t>
+          <t>George</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1385,23 +1525,28 @@
           <t>Team F</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>3</v>
       </c>
-      <c r="E29" t="n">
-        <v>66</v>
-      </c>
       <c r="F29" t="n">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G29" t="n">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H29" t="n">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="I29" t="n">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="J29" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="30">
@@ -1410,7 +1555,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Tammy</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1418,23 +1563,28 @@
           <t>Team F</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
         <v>4</v>
       </c>
-      <c r="E30" t="n">
-        <v>56</v>
-      </c>
       <c r="F30" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G30" t="n">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H30" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I30" t="n">
-        <v>56</v>
+        <v>38</v>
+      </c>
+      <c r="J30" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="31">
@@ -1443,7 +1593,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1451,23 +1601,28 @@
           <t>Team F</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
         <v>5</v>
       </c>
-      <c r="E31" t="n">
-        <v>56</v>
-      </c>
       <c r="F31" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G31" t="n">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H31" t="n">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="I31" t="n">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="J31" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="32">
@@ -1476,7 +1631,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1484,23 +1639,28 @@
           <t>Team G</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
         <v>1</v>
       </c>
-      <c r="E32" t="n">
-        <v>69</v>
-      </c>
       <c r="F32" t="n">
+        <v>48</v>
+      </c>
+      <c r="G32" t="n">
+        <v>52</v>
+      </c>
+      <c r="H32" t="n">
+        <v>49</v>
+      </c>
+      <c r="I32" t="n">
+        <v>73</v>
+      </c>
+      <c r="J32" t="n">
         <v>67</v>
-      </c>
-      <c r="G32" t="n">
-        <v>51</v>
-      </c>
-      <c r="H32" t="n">
-        <v>55</v>
-      </c>
-      <c r="I32" t="n">
-        <v>58</v>
       </c>
     </row>
     <row r="33">
@@ -1509,7 +1669,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Jeffrey</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1517,23 +1677,28 @@
           <t>Team G</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
         <v>2</v>
       </c>
-      <c r="E33" t="n">
-        <v>48</v>
-      </c>
       <c r="F33" t="n">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G33" t="n">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H33" t="n">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="I33" t="n">
-        <v>55</v>
+        <v>38</v>
+      </c>
+      <c r="J33" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="34">
@@ -1542,7 +1707,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Bryan</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1550,23 +1715,28 @@
           <t>Team G</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
         <v>3</v>
       </c>
-      <c r="E34" t="n">
-        <v>69</v>
-      </c>
       <c r="F34" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G34" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H34" t="n">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I34" t="n">
         <v>64</v>
+      </c>
+      <c r="J34" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="35">
@@ -1575,7 +1745,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Gene</t>
+          <t>Patsy</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1583,23 +1753,28 @@
           <t>Team G</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
         <v>4</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
+        <v>76</v>
+      </c>
+      <c r="G35" t="n">
+        <v>48</v>
+      </c>
+      <c r="H35" t="n">
+        <v>52</v>
+      </c>
+      <c r="I35" t="n">
         <v>59</v>
       </c>
-      <c r="F35" t="n">
-        <v>59</v>
-      </c>
-      <c r="G35" t="n">
-        <v>75</v>
-      </c>
-      <c r="H35" t="n">
-        <v>66</v>
-      </c>
-      <c r="I35" t="n">
-        <v>54</v>
+      <c r="J35" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="36">
@@ -1608,7 +1783,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Lora</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1616,23 +1791,28 @@
           <t>Team G</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
         <v>5</v>
       </c>
-      <c r="E36" t="n">
-        <v>80</v>
-      </c>
       <c r="F36" t="n">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G36" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H36" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I36" t="n">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="J36" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="37">
@@ -1641,7 +1821,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Karl</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1649,23 +1829,28 @@
           <t>Team H</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
         <v>1</v>
       </c>
-      <c r="E37" t="n">
-        <v>72</v>
-      </c>
       <c r="F37" t="n">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G37" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H37" t="n">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="I37" t="n">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="J37" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="38">
@@ -1674,7 +1859,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Minnie</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1682,23 +1867,28 @@
           <t>Team H</t>
         </is>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
         <v>2</v>
       </c>
-      <c r="E38" t="n">
-        <v>63</v>
-      </c>
       <c r="F38" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G38" t="n">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="H38" t="n">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="I38" t="n">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="J38" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="39">
@@ -1707,7 +1897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Heather</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1715,23 +1905,28 @@
           <t>Team H</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
         <v>3</v>
       </c>
-      <c r="E39" t="n">
-        <v>63</v>
-      </c>
       <c r="F39" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G39" t="n">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H39" t="n">
         <v>55</v>
       </c>
       <c r="I39" t="n">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="J39" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="40">
@@ -1740,7 +1935,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1748,23 +1943,28 @@
           <t>Team H</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
         <v>4</v>
       </c>
-      <c r="E40" t="n">
-        <v>62</v>
-      </c>
       <c r="F40" t="n">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="G40" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H40" t="n">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I40" t="n">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="J40" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="41">
@@ -1773,7 +1973,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1781,23 +1981,28 @@
           <t>Team H</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
         <v>5</v>
       </c>
-      <c r="E41" t="n">
-        <v>62</v>
-      </c>
       <c r="F41" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G41" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H41" t="n">
+        <v>67</v>
+      </c>
+      <c r="I41" t="n">
         <v>58</v>
       </c>
-      <c r="I41" t="n">
-        <v>68</v>
+      <c r="J41" t="n">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added stamina, fatigue and in line_up. preparations for substitutes
</commit_message>
<xml_diff>
--- a/players_excel.xlsx
+++ b/players_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>stability</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>stamina</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -491,7 +496,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fannie</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -508,19 +513,22 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2" t="n">
+        <v>58</v>
+      </c>
+      <c r="H2" t="n">
+        <v>62</v>
+      </c>
+      <c r="I2" t="n">
         <v>78</v>
       </c>
-      <c r="G2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H2" t="n">
-        <v>64</v>
-      </c>
-      <c r="I2" t="n">
-        <v>63</v>
-      </c>
       <c r="J2" t="n">
-        <v>60</v>
+        <v>86</v>
+      </c>
+      <c r="K2" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +537,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Carolyn</t>
+          <t>Allison</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -546,19 +554,22 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="G3" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="H3" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I3" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J3" t="n">
-        <v>53</v>
+        <v>62</v>
+      </c>
+      <c r="K3" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -567,7 +578,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lauren</t>
+          <t>Kelli</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -584,19 +595,22 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G4" t="n">
+        <v>64</v>
+      </c>
+      <c r="H4" t="n">
+        <v>77</v>
+      </c>
+      <c r="I4" t="n">
         <v>70</v>
       </c>
-      <c r="H4" t="n">
-        <v>66</v>
-      </c>
-      <c r="I4" t="n">
-        <v>78</v>
-      </c>
       <c r="J4" t="n">
-        <v>69</v>
+        <v>83</v>
+      </c>
+      <c r="K4" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="5">
@@ -605,7 +619,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Holly</t>
+          <t>Duane</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -622,19 +636,22 @@
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G5" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H5" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I5" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="J5" t="n">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="K5" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -643,7 +660,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wayne</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -660,19 +677,22 @@
         <v>5</v>
       </c>
       <c r="F6" t="n">
+        <v>62</v>
+      </c>
+      <c r="G6" t="n">
         <v>71</v>
       </c>
-      <c r="G6" t="n">
-        <v>67</v>
-      </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="I6" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="J6" t="n">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="K6" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="7">
@@ -681,7 +701,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Shayna</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -698,19 +718,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="G7" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H7" t="n">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="I7" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="J7" t="n">
-        <v>53</v>
+        <v>65</v>
+      </c>
+      <c r="K7" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -719,7 +742,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Howard</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -736,19 +759,22 @@
         <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G8" t="n">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H8" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="I8" t="n">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="J8" t="n">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="K8" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="9">
@@ -757,7 +783,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Deloris</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -774,19 +800,22 @@
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G9" t="n">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H9" t="n">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="I9" t="n">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J9" t="n">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="K9" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -795,7 +824,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -812,19 +841,22 @@
         <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G10" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H10" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I10" t="n">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="J10" t="n">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="K10" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -833,7 +865,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -850,19 +882,22 @@
         <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" t="n">
         <v>57</v>
       </c>
       <c r="H11" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I11" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J11" t="n">
-        <v>50</v>
+        <v>82</v>
+      </c>
+      <c r="K11" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="12">
@@ -871,7 +906,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Phyllis</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -888,19 +923,22 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" t="n">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H12" t="n">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="I12" t="n">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="J12" t="n">
-        <v>58</v>
+        <v>66</v>
+      </c>
+      <c r="K12" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -909,7 +947,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Felipe</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -926,19 +964,22 @@
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G13" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" t="n">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I13" t="n">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="J13" t="n">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="K13" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -947,7 +988,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Betty</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -964,19 +1005,22 @@
         <v>3</v>
       </c>
       <c r="F14" t="n">
+        <v>85</v>
+      </c>
+      <c r="G14" t="n">
+        <v>76</v>
+      </c>
+      <c r="H14" t="n">
+        <v>76</v>
+      </c>
+      <c r="I14" t="n">
+        <v>65</v>
+      </c>
+      <c r="J14" t="n">
         <v>56</v>
       </c>
-      <c r="G14" t="n">
-        <v>32</v>
-      </c>
-      <c r="H14" t="n">
-        <v>57</v>
-      </c>
-      <c r="I14" t="n">
-        <v>51</v>
-      </c>
-      <c r="J14" t="n">
-        <v>65</v>
+      <c r="K14" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -985,7 +1029,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ida</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1002,19 +1046,22 @@
         <v>4</v>
       </c>
       <c r="F15" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G15" t="n">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H15" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="I15" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J15" t="n">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="K15" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="16">
@@ -1023,7 +1070,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Crystal</t>
+          <t>Richard</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1040,19 +1087,22 @@
         <v>5</v>
       </c>
       <c r="F16" t="n">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="G16" t="n">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="H16" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I16" t="n">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="J16" t="n">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="K16" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="17">
@@ -1061,7 +1111,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ebony</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1078,19 +1128,22 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G17" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H17" t="n">
+        <v>72</v>
+      </c>
+      <c r="I17" t="n">
+        <v>62</v>
+      </c>
+      <c r="J17" t="n">
         <v>68</v>
       </c>
-      <c r="I17" t="n">
-        <v>52</v>
-      </c>
-      <c r="J17" t="n">
-        <v>64</v>
+      <c r="K17" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -1099,7 +1152,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Willis</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1116,10 +1169,10 @@
         <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G18" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="H18" t="n">
         <v>64</v>
@@ -1128,7 +1181,10 @@
         <v>65</v>
       </c>
       <c r="J18" t="n">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="K18" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -1137,7 +1193,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rachel</t>
+          <t>Kelli</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1154,19 +1210,22 @@
         <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G19" t="n">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="H19" t="n">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I19" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J19" t="n">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="K19" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="20">
@@ -1175,7 +1234,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1192,19 +1251,22 @@
         <v>4</v>
       </c>
       <c r="F20" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="G20" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H20" t="n">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="I20" t="n">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="J20" t="n">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="K20" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="21">
@@ -1213,7 +1275,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1230,19 +1292,22 @@
         <v>5</v>
       </c>
       <c r="F21" t="n">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="G21" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H21" t="n">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="I21" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J21" t="n">
-        <v>55</v>
+        <v>71</v>
+      </c>
+      <c r="K21" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="22">
@@ -1251,7 +1316,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jacob</t>
+          <t>Annie</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1268,19 +1333,22 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="G22" t="n">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H22" t="n">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I22" t="n">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="J22" t="n">
-        <v>40</v>
+        <v>69</v>
+      </c>
+      <c r="K22" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="23">
@@ -1289,7 +1357,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Edward</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1306,19 +1374,22 @@
         <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G23" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" t="n">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="I23" t="n">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="J23" t="n">
         <v>70</v>
+      </c>
+      <c r="K23" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="24">
@@ -1327,7 +1398,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>Walter</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1344,19 +1415,22 @@
         <v>3</v>
       </c>
       <c r="F24" t="n">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="G24" t="n">
+        <v>66</v>
+      </c>
+      <c r="H24" t="n">
+        <v>73</v>
+      </c>
+      <c r="I24" t="n">
+        <v>56</v>
+      </c>
+      <c r="J24" t="n">
         <v>63</v>
       </c>
-      <c r="H24" t="n">
-        <v>77</v>
-      </c>
-      <c r="I24" t="n">
-        <v>54</v>
-      </c>
-      <c r="J24" t="n">
-        <v>59</v>
+      <c r="K24" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="25">
@@ -1365,7 +1439,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1382,19 +1456,22 @@
         <v>4</v>
       </c>
       <c r="F25" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G25" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H25" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="I25" t="n">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="J25" t="n">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="K25" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="26">
@@ -1403,7 +1480,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Olive</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1420,19 +1497,22 @@
         <v>5</v>
       </c>
       <c r="F26" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G26" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H26" t="n">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="I26" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="J26" t="n">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="K26" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="27">
@@ -1441,7 +1521,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Debra</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1458,19 +1538,22 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="G27" t="n">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="H27" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I27" t="n">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="J27" t="n">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="K27" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="28">
@@ -1479,7 +1562,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Christine</t>
+          <t>Bonnie</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1496,19 +1579,22 @@
         <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G28" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H28" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I28" t="n">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="J28" t="n">
-        <v>62</v>
+        <v>88</v>
+      </c>
+      <c r="K28" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="29">
@@ -1517,7 +1603,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Sylvia</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1534,19 +1620,22 @@
         <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G29" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H29" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="I29" t="n">
+        <v>72</v>
+      </c>
+      <c r="J29" t="n">
+        <v>78</v>
+      </c>
+      <c r="K29" t="n">
         <v>61</v>
-      </c>
-      <c r="J29" t="n">
-        <v>67</v>
       </c>
     </row>
     <row r="30">
@@ -1555,7 +1644,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Brooke</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1572,19 +1661,22 @@
         <v>4</v>
       </c>
       <c r="F30" t="n">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="G30" t="n">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="H30" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="I30" t="n">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="J30" t="n">
-        <v>71</v>
+        <v>62</v>
+      </c>
+      <c r="K30" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="31">
@@ -1593,7 +1685,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Janet</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1610,19 +1702,22 @@
         <v>5</v>
       </c>
       <c r="F31" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G31" t="n">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="H31" t="n">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="I31" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="J31" t="n">
-        <v>46</v>
+        <v>80</v>
+      </c>
+      <c r="K31" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="32">
@@ -1631,7 +1726,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Felicia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1648,19 +1743,22 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="G32" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H32" t="n">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="I32" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J32" t="n">
-        <v>67</v>
+        <v>87</v>
+      </c>
+      <c r="K32" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="33">
@@ -1669,7 +1767,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1686,19 +1784,22 @@
         <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G33" t="n">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H33" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I33" t="n">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="J33" t="n">
-        <v>54</v>
+        <v>71</v>
+      </c>
+      <c r="K33" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="34">
@@ -1707,7 +1808,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bryan</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1724,19 +1825,22 @@
         <v>3</v>
       </c>
       <c r="F34" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G34" t="n">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H34" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I34" t="n">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="J34" t="n">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="K34" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="35">
@@ -1745,7 +1849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Patsy</t>
+          <t>Muriel</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1762,19 +1866,22 @@
         <v>4</v>
       </c>
       <c r="F35" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G35" t="n">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="H35" t="n">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="I35" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="J35" t="n">
-        <v>74</v>
+        <v>39</v>
+      </c>
+      <c r="K35" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="36">
@@ -1783,7 +1890,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lora</t>
+          <t>Sadie</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1800,19 +1907,22 @@
         <v>5</v>
       </c>
       <c r="F36" t="n">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="G36" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="H36" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I36" t="n">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="J36" t="n">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="K36" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="37">
@@ -1838,19 +1948,22 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="G37" t="n">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="H37" t="n">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="I37" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="J37" t="n">
-        <v>44</v>
+        <v>78</v>
+      </c>
+      <c r="K37" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="38">
@@ -1859,7 +1972,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Minnie</t>
+          <t>Dale</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1876,19 +1989,22 @@
         <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G38" t="n">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H38" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="I38" t="n">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J38" t="n">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="K38" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="39">
@@ -1897,7 +2013,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1914,19 +2030,22 @@
         <v>3</v>
       </c>
       <c r="F39" t="n">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G39" t="n">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H39" t="n">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I39" t="n">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="J39" t="n">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="K39" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="40">
@@ -1935,7 +2054,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1955,16 +2074,19 @@
         <v>69</v>
       </c>
       <c r="G40" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H40" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I40" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="J40" t="n">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="K40" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="41">
@@ -1973,7 +2095,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1990,19 +2112,22 @@
         <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="G41" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H41" t="n">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I41" t="n">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="J41" t="n">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="K41" t="n">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
find_top_players moved to data league ranking evaluates ratio as secondary parameter 8 players in team fixing print top team
</commit_message>
<xml_diff>
--- a/players_excel.xlsx
+++ b/players_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Judith</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -513,22 +513,22 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="G2" t="n">
+        <v>63</v>
+      </c>
+      <c r="H2" t="n">
+        <v>71</v>
+      </c>
+      <c r="I2" t="n">
         <v>58</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>62</v>
       </c>
-      <c r="I2" t="n">
-        <v>78</v>
-      </c>
-      <c r="J2" t="n">
-        <v>86</v>
-      </c>
       <c r="K2" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Allison</t>
+          <t>Elvin</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,22 +554,22 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G3" t="n">
+        <v>61</v>
+      </c>
+      <c r="H3" t="n">
+        <v>71</v>
+      </c>
+      <c r="I3" t="n">
         <v>65</v>
       </c>
-      <c r="H3" t="n">
-        <v>75</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
+        <v>74</v>
+      </c>
+      <c r="K3" t="n">
         <v>63</v>
-      </c>
-      <c r="J3" t="n">
-        <v>62</v>
-      </c>
-      <c r="K3" t="n">
-        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -578,7 +578,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kelli</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -595,22 +595,22 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G4" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H4" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I4" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="J4" t="n">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="K4" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -619,7 +619,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Duane</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -636,22 +636,22 @@
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G5" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H5" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I5" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J5" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K5" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
@@ -660,7 +660,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Kendra</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -677,22 +677,22 @@
         <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G6" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H6" t="n">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="I6" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="J6" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" t="n">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -701,39 +701,39 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Team B</t>
+          <t>Team A</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>blue</t>
+          <t>red</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G7" t="n">
+        <v>58</v>
+      </c>
+      <c r="H7" t="n">
+        <v>66</v>
+      </c>
+      <c r="I7" t="n">
+        <v>64</v>
+      </c>
+      <c r="J7" t="n">
+        <v>71</v>
+      </c>
+      <c r="K7" t="n">
         <v>54</v>
-      </c>
-      <c r="H7" t="n">
-        <v>73</v>
-      </c>
-      <c r="I7" t="n">
-        <v>75</v>
-      </c>
-      <c r="J7" t="n">
-        <v>65</v>
-      </c>
-      <c r="K7" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -742,39 +742,39 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Veronica</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Team B</t>
+          <t>Team A</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>blue</t>
+          <t>red</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G8" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H8" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I8" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J8" t="n">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K8" t="n">
-        <v>77</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -783,39 +783,39 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Team B</t>
+          <t>Team A</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>blue</t>
+          <t>red</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G9" t="n">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="H9" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="I9" t="n">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J9" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K9" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
@@ -824,7 +824,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Anthony</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -838,25 +838,25 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
+        <v>69</v>
+      </c>
+      <c r="G10" t="n">
+        <v>72</v>
+      </c>
+      <c r="H10" t="n">
+        <v>64</v>
+      </c>
+      <c r="I10" t="n">
+        <v>59</v>
+      </c>
+      <c r="J10" t="n">
+        <v>57</v>
+      </c>
+      <c r="K10" t="n">
         <v>56</v>
-      </c>
-      <c r="G10" t="n">
-        <v>85</v>
-      </c>
-      <c r="H10" t="n">
-        <v>66</v>
-      </c>
-      <c r="I10" t="n">
-        <v>76</v>
-      </c>
-      <c r="J10" t="n">
-        <v>70</v>
-      </c>
-      <c r="K10" t="n">
-        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -865,7 +865,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Adam</t>
+          <t>Anthony</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -879,25 +879,25 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="G11" t="n">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H11" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I11" t="n">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K11" t="n">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
@@ -906,33 +906,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Team C</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G12" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H12" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I12" t="n">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="J12" t="n">
         <v>66</v>
@@ -947,39 +947,39 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Team C</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
+        <v>45</v>
+      </c>
+      <c r="G13" t="n">
+        <v>62</v>
+      </c>
+      <c r="H13" t="n">
+        <v>66</v>
+      </c>
+      <c r="I13" t="n">
+        <v>73</v>
+      </c>
+      <c r="J13" t="n">
         <v>70</v>
       </c>
-      <c r="G13" t="n">
-        <v>61</v>
-      </c>
-      <c r="H13" t="n">
-        <v>73</v>
-      </c>
-      <c r="I13" t="n">
-        <v>76</v>
-      </c>
-      <c r="J13" t="n">
-        <v>69</v>
-      </c>
       <c r="K13" t="n">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
@@ -988,39 +988,39 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Rachael</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Team C</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G14" t="n">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="H14" t="n">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="I14" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J14" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="K14" t="n">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -1029,39 +1029,39 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Team C</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G15" t="n">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H15" t="n">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="I15" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J15" t="n">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="K15" t="n">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -1070,39 +1070,39 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Team C</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G16" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H16" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I16" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="J16" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K16" t="n">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -1111,39 +1111,39 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Althea</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Team D</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G17" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H17" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I17" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="J17" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K17" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -1152,39 +1152,39 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Willis</t>
+          <t>Stephaine</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Team D</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G18" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H18" t="n">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I18" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J18" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K18" t="n">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
@@ -1193,39 +1193,39 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kelli</t>
+          <t>Isabell</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Team D</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="G19" t="n">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="H19" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="I19" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="J19" t="n">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="K19" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20">
@@ -1234,36 +1234,36 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Kenneth</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Team D</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G20" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="H20" t="n">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="I20" t="n">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="J20" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K20" t="n">
         <v>69</v>
@@ -1275,39 +1275,39 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Team D</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G21" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H21" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I21" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="J21" t="n">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="K21" t="n">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
@@ -1316,39 +1316,39 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Annie</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Team E</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>magenta</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G22" t="n">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H22" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I22" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J22" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="K22" t="n">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23">
@@ -1357,39 +1357,39 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Edward</t>
+          <t>Samantha</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Team E</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>magenta</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G23" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H23" t="n">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="I23" t="n">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="J23" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="K23" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
@@ -1398,39 +1398,39 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Walter</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Team E</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>magenta</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G24" t="n">
+        <v>59</v>
+      </c>
+      <c r="H24" t="n">
         <v>66</v>
       </c>
-      <c r="H24" t="n">
-        <v>73</v>
-      </c>
       <c r="I24" t="n">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="J24" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K24" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
@@ -1439,39 +1439,39 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Julie</t>
+          <t>Keith</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Team E</t>
+          <t>Team C</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>magenta</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="G25" t="n">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="H25" t="n">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="I25" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="J25" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K25" t="n">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26">
@@ -1480,39 +1480,39 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Olive</t>
+          <t>Jerome</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Team E</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>magenta</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G26" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H26" t="n">
+        <v>55</v>
+      </c>
+      <c r="I26" t="n">
         <v>68</v>
       </c>
-      <c r="I26" t="n">
-        <v>72</v>
-      </c>
       <c r="J26" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K26" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27">
@@ -1521,36 +1521,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Debra</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Team F</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G27" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H27" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I27" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J27" t="n">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="K27" t="n">
         <v>69</v>
@@ -1562,39 +1562,39 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bonnie</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Team F</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G28" t="n">
+        <v>45</v>
+      </c>
+      <c r="H28" t="n">
+        <v>65</v>
+      </c>
+      <c r="I28" t="n">
+        <v>59</v>
+      </c>
+      <c r="J28" t="n">
+        <v>71</v>
+      </c>
+      <c r="K28" t="n">
         <v>75</v>
-      </c>
-      <c r="H28" t="n">
-        <v>55</v>
-      </c>
-      <c r="I28" t="n">
-        <v>65</v>
-      </c>
-      <c r="J28" t="n">
-        <v>88</v>
-      </c>
-      <c r="K28" t="n">
-        <v>76</v>
       </c>
     </row>
     <row r="29">
@@ -1603,39 +1603,39 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sylvia</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Team F</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G29" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H29" t="n">
+        <v>68</v>
+      </c>
+      <c r="I29" t="n">
         <v>63</v>
       </c>
-      <c r="I29" t="n">
-        <v>72</v>
-      </c>
       <c r="J29" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="K29" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30">
@@ -1644,39 +1644,39 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Brooke</t>
+          <t>Carrie</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Team F</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G30" t="n">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H30" t="n">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="I30" t="n">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="J30" t="n">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K30" t="n">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">
@@ -1685,39 +1685,39 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Team F</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G31" t="n">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="H31" t="n">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="I31" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="J31" t="n">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K31" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
@@ -1726,39 +1726,39 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Felicia</t>
+          <t>Joanna</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Team G</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>gray</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G32" t="n">
+        <v>69</v>
+      </c>
+      <c r="H32" t="n">
+        <v>42</v>
+      </c>
+      <c r="I32" t="n">
         <v>59</v>
       </c>
-      <c r="H32" t="n">
-        <v>83</v>
-      </c>
-      <c r="I32" t="n">
-        <v>71</v>
-      </c>
       <c r="J32" t="n">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K32" t="n">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
@@ -1767,39 +1767,39 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Wilfred</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Team G</t>
+          <t>Team D</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>gray</t>
+          <t>yellow</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="G33" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H33" t="n">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="I33" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J33" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K33" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34">
@@ -1808,39 +1808,39 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Team G</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>gray</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
+        <v>70</v>
+      </c>
+      <c r="G34" t="n">
+        <v>74</v>
+      </c>
+      <c r="H34" t="n">
+        <v>63</v>
+      </c>
+      <c r="I34" t="n">
         <v>68</v>
       </c>
-      <c r="G34" t="n">
-        <v>71</v>
-      </c>
-      <c r="H34" t="n">
-        <v>60</v>
-      </c>
-      <c r="I34" t="n">
-        <v>82</v>
-      </c>
       <c r="J34" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="K34" t="n">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35">
@@ -1849,39 +1849,39 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Muriel</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Team G</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>gray</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G35" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="H35" t="n">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="I35" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J35" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K35" t="n">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36">
@@ -1890,39 +1890,39 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sadie</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Team G</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>gray</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G36" t="n">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H36" t="n">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="I36" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="J36" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="K36" t="n">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37">
@@ -1931,39 +1931,39 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Team H</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G37" t="n">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H37" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="I37" t="n">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="J37" t="n">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="K37" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38">
@@ -1972,39 +1972,39 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dale</t>
+          <t>Verna</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Team H</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="G38" t="n">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H38" t="n">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="I38" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J38" t="n">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="K38" t="n">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39">
@@ -2013,39 +2013,39 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Cherie</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Team H</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G39" t="n">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H39" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I39" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="J39" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K39" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40">
@@ -2054,39 +2054,39 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Jon</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Team H</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G40" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H40" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I40" t="n">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="J40" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="K40" t="n">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41">
@@ -2095,39 +2095,1023 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Lucile</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Team H</t>
+          <t>Team E</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>magenta</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F41" t="n">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="G41" t="n">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="H41" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="I41" t="n">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="J41" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K41" t="n">
         <v>61</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>51</v>
+      </c>
+      <c r="G42" t="n">
+        <v>69</v>
+      </c>
+      <c r="H42" t="n">
+        <v>69</v>
+      </c>
+      <c r="I42" t="n">
+        <v>73</v>
+      </c>
+      <c r="J42" t="n">
+        <v>74</v>
+      </c>
+      <c r="K42" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>74</v>
+      </c>
+      <c r="G43" t="n">
+        <v>59</v>
+      </c>
+      <c r="H43" t="n">
+        <v>54</v>
+      </c>
+      <c r="I43" t="n">
+        <v>65</v>
+      </c>
+      <c r="J43" t="n">
+        <v>70</v>
+      </c>
+      <c r="K43" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Sally</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" t="n">
+        <v>25</v>
+      </c>
+      <c r="G44" t="n">
+        <v>61</v>
+      </c>
+      <c r="H44" t="n">
+        <v>74</v>
+      </c>
+      <c r="I44" t="n">
+        <v>62</v>
+      </c>
+      <c r="J44" t="n">
+        <v>64</v>
+      </c>
+      <c r="K44" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Stephanie</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>4</v>
+      </c>
+      <c r="F45" t="n">
+        <v>54</v>
+      </c>
+      <c r="G45" t="n">
+        <v>71</v>
+      </c>
+      <c r="H45" t="n">
+        <v>64</v>
+      </c>
+      <c r="I45" t="n">
+        <v>64</v>
+      </c>
+      <c r="J45" t="n">
+        <v>59</v>
+      </c>
+      <c r="K45" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Carol</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>5</v>
+      </c>
+      <c r="F46" t="n">
+        <v>67</v>
+      </c>
+      <c r="G46" t="n">
+        <v>52</v>
+      </c>
+      <c r="H46" t="n">
+        <v>72</v>
+      </c>
+      <c r="I46" t="n">
+        <v>66</v>
+      </c>
+      <c r="J46" t="n">
+        <v>59</v>
+      </c>
+      <c r="K46" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>6</v>
+      </c>
+      <c r="F47" t="n">
+        <v>72</v>
+      </c>
+      <c r="G47" t="n">
+        <v>59</v>
+      </c>
+      <c r="H47" t="n">
+        <v>70</v>
+      </c>
+      <c r="I47" t="n">
+        <v>61</v>
+      </c>
+      <c r="J47" t="n">
+        <v>59</v>
+      </c>
+      <c r="K47" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Bella</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>7</v>
+      </c>
+      <c r="F48" t="n">
+        <v>71</v>
+      </c>
+      <c r="G48" t="n">
+        <v>50</v>
+      </c>
+      <c r="H48" t="n">
+        <v>61</v>
+      </c>
+      <c r="I48" t="n">
+        <v>77</v>
+      </c>
+      <c r="J48" t="n">
+        <v>72</v>
+      </c>
+      <c r="K48" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Carl</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Team F</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>8</v>
+      </c>
+      <c r="F49" t="n">
+        <v>57</v>
+      </c>
+      <c r="G49" t="n">
+        <v>59</v>
+      </c>
+      <c r="H49" t="n">
+        <v>73</v>
+      </c>
+      <c r="I49" t="n">
+        <v>62</v>
+      </c>
+      <c r="J49" t="n">
+        <v>62</v>
+      </c>
+      <c r="K49" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dustin</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>63</v>
+      </c>
+      <c r="G50" t="n">
+        <v>83</v>
+      </c>
+      <c r="H50" t="n">
+        <v>56</v>
+      </c>
+      <c r="I50" t="n">
+        <v>82</v>
+      </c>
+      <c r="J50" t="n">
+        <v>59</v>
+      </c>
+      <c r="K50" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Billie</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" t="n">
+        <v>61</v>
+      </c>
+      <c r="G51" t="n">
+        <v>78</v>
+      </c>
+      <c r="H51" t="n">
+        <v>64</v>
+      </c>
+      <c r="I51" t="n">
+        <v>67</v>
+      </c>
+      <c r="J51" t="n">
+        <v>65</v>
+      </c>
+      <c r="K51" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>3</v>
+      </c>
+      <c r="F52" t="n">
+        <v>62</v>
+      </c>
+      <c r="G52" t="n">
+        <v>65</v>
+      </c>
+      <c r="H52" t="n">
+        <v>61</v>
+      </c>
+      <c r="I52" t="n">
+        <v>68</v>
+      </c>
+      <c r="J52" t="n">
+        <v>66</v>
+      </c>
+      <c r="K52" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Carl</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>4</v>
+      </c>
+      <c r="F53" t="n">
+        <v>90</v>
+      </c>
+      <c r="G53" t="n">
+        <v>64</v>
+      </c>
+      <c r="H53" t="n">
+        <v>58</v>
+      </c>
+      <c r="I53" t="n">
+        <v>53</v>
+      </c>
+      <c r="J53" t="n">
+        <v>59</v>
+      </c>
+      <c r="K53" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Pearl</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>5</v>
+      </c>
+      <c r="F54" t="n">
+        <v>61</v>
+      </c>
+      <c r="G54" t="n">
+        <v>65</v>
+      </c>
+      <c r="H54" t="n">
+        <v>76</v>
+      </c>
+      <c r="I54" t="n">
+        <v>81</v>
+      </c>
+      <c r="J54" t="n">
+        <v>76</v>
+      </c>
+      <c r="K54" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Frances</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>6</v>
+      </c>
+      <c r="F55" t="n">
+        <v>73</v>
+      </c>
+      <c r="G55" t="n">
+        <v>75</v>
+      </c>
+      <c r="H55" t="n">
+        <v>62</v>
+      </c>
+      <c r="I55" t="n">
+        <v>58</v>
+      </c>
+      <c r="J55" t="n">
+        <v>54</v>
+      </c>
+      <c r="K55" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Gilbert</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>7</v>
+      </c>
+      <c r="F56" t="n">
+        <v>65</v>
+      </c>
+      <c r="G56" t="n">
+        <v>78</v>
+      </c>
+      <c r="H56" t="n">
+        <v>70</v>
+      </c>
+      <c r="I56" t="n">
+        <v>48</v>
+      </c>
+      <c r="J56" t="n">
+        <v>85</v>
+      </c>
+      <c r="K56" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Ruby</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Team G</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>8</v>
+      </c>
+      <c r="F57" t="n">
+        <v>54</v>
+      </c>
+      <c r="G57" t="n">
+        <v>63</v>
+      </c>
+      <c r="H57" t="n">
+        <v>68</v>
+      </c>
+      <c r="I57" t="n">
+        <v>74</v>
+      </c>
+      <c r="J57" t="n">
+        <v>49</v>
+      </c>
+      <c r="K57" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>51</v>
+      </c>
+      <c r="G58" t="n">
+        <v>53</v>
+      </c>
+      <c r="H58" t="n">
+        <v>61</v>
+      </c>
+      <c r="I58" t="n">
+        <v>58</v>
+      </c>
+      <c r="J58" t="n">
+        <v>62</v>
+      </c>
+      <c r="K58" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="n">
+        <v>65</v>
+      </c>
+      <c r="G59" t="n">
+        <v>57</v>
+      </c>
+      <c r="H59" t="n">
+        <v>84</v>
+      </c>
+      <c r="I59" t="n">
+        <v>58</v>
+      </c>
+      <c r="J59" t="n">
+        <v>82</v>
+      </c>
+      <c r="K59" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="n">
+        <v>59</v>
+      </c>
+      <c r="G60" t="n">
+        <v>68</v>
+      </c>
+      <c r="H60" t="n">
+        <v>77</v>
+      </c>
+      <c r="I60" t="n">
+        <v>50</v>
+      </c>
+      <c r="J60" t="n">
+        <v>73</v>
+      </c>
+      <c r="K60" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Rosemary</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>4</v>
+      </c>
+      <c r="F61" t="n">
+        <v>75</v>
+      </c>
+      <c r="G61" t="n">
+        <v>66</v>
+      </c>
+      <c r="H61" t="n">
+        <v>62</v>
+      </c>
+      <c r="I61" t="n">
+        <v>69</v>
+      </c>
+      <c r="J61" t="n">
+        <v>71</v>
+      </c>
+      <c r="K61" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>5</v>
+      </c>
+      <c r="F62" t="n">
+        <v>51</v>
+      </c>
+      <c r="G62" t="n">
+        <v>80</v>
+      </c>
+      <c r="H62" t="n">
+        <v>57</v>
+      </c>
+      <c r="I62" t="n">
+        <v>70</v>
+      </c>
+      <c r="J62" t="n">
+        <v>52</v>
+      </c>
+      <c r="K62" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>6</v>
+      </c>
+      <c r="F63" t="n">
+        <v>40</v>
+      </c>
+      <c r="G63" t="n">
+        <v>65</v>
+      </c>
+      <c r="H63" t="n">
+        <v>56</v>
+      </c>
+      <c r="I63" t="n">
+        <v>78</v>
+      </c>
+      <c r="J63" t="n">
+        <v>55</v>
+      </c>
+      <c r="K63" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Derrick</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>7</v>
+      </c>
+      <c r="F64" t="n">
+        <v>75</v>
+      </c>
+      <c r="G64" t="n">
+        <v>76</v>
+      </c>
+      <c r="H64" t="n">
+        <v>52</v>
+      </c>
+      <c r="I64" t="n">
+        <v>65</v>
+      </c>
+      <c r="J64" t="n">
+        <v>50</v>
+      </c>
+      <c r="K64" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Joy</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Team H</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>8</v>
+      </c>
+      <c r="F65" t="n">
+        <v>61</v>
+      </c>
+      <c r="G65" t="n">
+        <v>66</v>
+      </c>
+      <c r="H65" t="n">
+        <v>51</v>
+      </c>
+      <c r="I65" t="n">
+        <v>69</v>
+      </c>
+      <c r="J65" t="n">
+        <v>65</v>
+      </c>
+      <c r="K65" t="n">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>